<commit_message>
Feat: RE Place "\n"
</commit_message>
<xml_diff>
--- a/Assets/JA/MoveSystem/Scripts/PlaceDialogDB.xlsx
+++ b/Assets/JA/MoveSystem/Scripts/PlaceDialogDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\Bridge_Project_git\Assets\JA\MoveSystem\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E7CE23-2CFC-40B0-828C-4B7A6CC7ABB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B068A0-AAEB-4464-9AA5-DA6CFE9214B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61B2A508-873C-4A1A-9A46-20A497CA35A5}"/>
+    <workbookView xWindow="6045" yWindow="1005" windowWidth="21600" windowHeight="13800" xr2:uid="{61B2A508-873C-4A1A-9A46-20A497CA35A5}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaceEntity" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -163,38 +163,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아론</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aron_Happy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aron_Sad</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포키</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F_Happy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F_Sad</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나는 에프</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>킬라입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TreeImageType01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -221,13 +189,58 @@
   <si>
     <t>c</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(사람들의 대화 소리가 들린다.)</t>
+  </si>
+  <si>
+    <t>TreeButton</t>
+  </si>
+  <si>
+    <t>TreeImageType00</t>
+  </si>
+  <si>
+    <t>인물A</t>
+  </si>
+  <si>
+    <t>Lorena_Happy</t>
+  </si>
+  <si>
+    <t>이 나무 엄청 커! 왜 이렇게 큰거야??</t>
+  </si>
+  <si>
+    <t>인물B</t>
+  </si>
+  <si>
+    <t>중앙 나무를 이렇게 가까이에서 본 적은 처음이지?</t>
+  </si>
+  <si>
+    <t>이 나무는 세상에서 가장 오래된 나무야.\n그 긴 세월 동안 비가 오나 눈이 오나 이 자리를 지켜준 소중한 나무지.</t>
+  </si>
+  <si>
+    <t>이 나무 덕분에 사람들이 모이고, 지금 이렇게 트리안이 있을 수 있는 거란다.</t>
+  </si>
+  <si>
+    <t>와! 그냥 엄청 큰 나무인줄로만 알았어요!</t>
+  </si>
+  <si>
+    <t>하늘에 닿을 만큼 크기도 하지만, 이 나무는 트리안의 소중한 친구지.</t>
+  </si>
+  <si>
+    <t>이 나무만 근처에만 있으면 마음이 편안해지지 않니?</t>
+  </si>
+  <si>
+    <t>음... 기분 좋은 향이 나!</t>
+  </si>
+  <si>
+    <t>(나무가 바람에 흔들리는 소리)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,21 +269,63 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="double">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -279,9 +334,27 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B58999-3F71-4D9F-A862-1DDFFCC6D8C9}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -846,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -860,256 +933,248 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="B22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" t="b">
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1171,13 +1236,13 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -1188,13 +1253,13 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1205,13 +1270,13 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -1244,16 +1309,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1274,5 +1339,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: Dialogue Typing Text Add
</commit_message>
<xml_diff>
--- a/Assets/JA/MoveSystem/Scripts/PlaceDialogDB.xlsx
+++ b/Assets/JA/MoveSystem/Scripts/PlaceDialogDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\Bridge_Project_git\Assets\JA\MoveSystem\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B068A0-AAEB-4464-9AA5-DA6CFE9214B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024BDF5E-5308-4FB8-8B1C-1019B378B3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="1005" windowWidth="21600" windowHeight="13800" xr2:uid="{61B2A508-873C-4A1A-9A46-20A497CA35A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{61B2A508-873C-4A1A-9A46-20A497CA35A5}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaceEntity" sheetId="3" r:id="rId1"/>
@@ -673,7 +673,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -982,8 +982,8 @@
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>39</v>
+      <c r="C15" t="s">
+        <v>6</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>42</v>
@@ -1028,8 +1028,8 @@
       <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>39</v>
+      <c r="C17" t="s">
+        <v>6</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>43</v>
@@ -1051,8 +1051,8 @@
       <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
+      <c r="C18" t="s">
+        <v>6</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>44</v>
@@ -1097,8 +1097,8 @@
       <c r="B20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>39</v>
+      <c r="C20" t="s">
+        <v>6</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>46</v>
@@ -1120,8 +1120,8 @@
       <c r="B21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>39</v>
+      <c r="C21" t="s">
+        <v>6</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>47</v>

</xml_diff>